<commit_message>
add 'tool' node and its relationship
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\1 学习资料\9-大四上\制造工艺设计实践\202221106-knowlegeGraph\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7515B233-32A4-45B9-9B23-74FF74710561}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F45B2C3B-1C8A-40A1-A4B3-E02886F7323F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8184" yWindow="156" windowWidth="12156" windowHeight="12192" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="nodeData" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="133">
   <si>
     <t>label</t>
   </si>
@@ -122,9 +122,6 @@
     <t>精镗</t>
   </si>
   <si>
-    <t>落地镗铣床</t>
-  </si>
-  <si>
     <t>粗磨</t>
   </si>
   <si>
@@ -161,9 +158,6 @@
     <t>半精铣</t>
   </si>
   <si>
-    <t>单柱铣床</t>
-  </si>
-  <si>
     <t>精铣</t>
   </si>
   <si>
@@ -176,9 +170,6 @@
     <t>高速精铣</t>
   </si>
   <si>
-    <t>单柱刨床</t>
-  </si>
-  <si>
     <t>最大刨削宽度</t>
   </si>
   <si>
@@ -212,9 +203,6 @@
     <t>刮研</t>
   </si>
   <si>
-    <t>螺纹磨床</t>
-  </si>
-  <si>
     <t>粗车</t>
   </si>
   <si>
@@ -272,9 +260,6 @@
     <t>珩磨</t>
   </si>
   <si>
-    <t>待定</t>
-  </si>
-  <si>
     <t>圆板牙套</t>
   </si>
   <si>
@@ -327,13 +312,155 @@
   </si>
   <si>
     <t>可用设备</t>
+  </si>
+  <si>
+    <t>龙门铣床</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>高速铣床</t>
+  </si>
+  <si>
+    <t>高速铣床</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>龙门刨床</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>宽刀精刨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>label</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tool</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>外圆车刀</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>镗孔车刀</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>端面车刀</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>切断车刀</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>切槽车刀</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>螺纹车刀</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>麻花钻</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>扩孔钻</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>机用铰刀</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>手用铰刀</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>面铣刀</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>立铣刀</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>槽铣刀</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>键槽铣刀</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>粗加工用拉刀</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>精加工用拉刀</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>砂轮</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>装备刀具</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>手工</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>牛头刨床</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>刨刀</t>
+  </si>
+  <si>
+    <t>推荐刀具</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>钻孔</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>扩孔</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>铰孔</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>手铰</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>粗拉</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>精拉</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -347,6 +474,12 @@
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -369,8 +502,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -651,10 +785,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O38"/>
+  <dimension ref="A1:Q38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="Q19" sqref="Q19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -663,9 +797,11 @@
     <col min="3" max="3" width="8.88671875" customWidth="1"/>
     <col min="9" max="9" width="10.109375" customWidth="1"/>
     <col min="10" max="10" width="17.5546875" customWidth="1"/>
+    <col min="15" max="15" width="15" customWidth="1"/>
+    <col min="17" max="17" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -711,8 +847,14 @@
       <c r="O1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P1" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -758,8 +900,14 @@
       <c r="O2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P2" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -805,8 +953,14 @@
       <c r="O3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P3" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -852,8 +1006,14 @@
       <c r="O4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P4" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -899,8 +1059,14 @@
       <c r="O5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P5" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -946,8 +1112,14 @@
       <c r="O6" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P6" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>11</v>
       </c>
@@ -987,8 +1159,14 @@
       <c r="O7" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P7" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>11</v>
       </c>
@@ -1011,30 +1189,30 @@
         <v>13</v>
       </c>
       <c r="J8" t="s">
+        <v>34</v>
+      </c>
+      <c r="K8">
+        <v>200</v>
+      </c>
+      <c r="L8">
+        <v>630</v>
+      </c>
+      <c r="O8" t="s">
+        <v>35</v>
+      </c>
+      <c r="P8" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" t="s">
         <v>33</v>
-      </c>
-      <c r="K8">
-        <v>130</v>
-      </c>
-      <c r="L8">
-        <v>260</v>
-      </c>
-      <c r="M8">
-        <v>7</v>
-      </c>
-      <c r="N8">
-        <v>8</v>
-      </c>
-      <c r="O8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" t="s">
-        <v>34</v>
       </c>
       <c r="E9">
         <v>9</v>
@@ -1052,24 +1230,30 @@
         <v>13</v>
       </c>
       <c r="J9" t="s">
+        <v>37</v>
+      </c>
+      <c r="K9">
+        <v>630</v>
+      </c>
+      <c r="L9">
+        <v>2000</v>
+      </c>
+      <c r="O9" t="s">
         <v>35</v>
       </c>
-      <c r="K9">
-        <v>200</v>
-      </c>
-      <c r="L9">
-        <v>630</v>
-      </c>
-      <c r="O9" t="s">
+      <c r="P9" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" t="s">
         <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" t="s">
-        <v>37</v>
       </c>
       <c r="E10">
         <v>7</v>
@@ -1087,24 +1271,36 @@
         <v>13</v>
       </c>
       <c r="J10" t="s">
+        <v>39</v>
+      </c>
+      <c r="K10">
+        <v>250</v>
+      </c>
+      <c r="L10">
+        <v>620</v>
+      </c>
+      <c r="M10">
+        <v>5</v>
+      </c>
+      <c r="N10">
+        <v>7</v>
+      </c>
+      <c r="O10" t="s">
+        <v>35</v>
+      </c>
+      <c r="P10" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" t="s">
         <v>38</v>
-      </c>
-      <c r="K10">
-        <v>630</v>
-      </c>
-      <c r="L10">
-        <v>2000</v>
-      </c>
-      <c r="O10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" t="s">
-        <v>39</v>
       </c>
       <c r="E11">
         <v>9</v>
@@ -1122,30 +1318,36 @@
         <v>13</v>
       </c>
       <c r="J11" t="s">
+        <v>41</v>
+      </c>
+      <c r="K11">
+        <v>200</v>
+      </c>
+      <c r="L11">
+        <v>500</v>
+      </c>
+      <c r="M11">
+        <v>8</v>
+      </c>
+      <c r="N11">
+        <v>9</v>
+      </c>
+      <c r="O11" t="s">
+        <v>35</v>
+      </c>
+      <c r="P11" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" t="s">
         <v>40</v>
-      </c>
-      <c r="K11">
-        <v>250</v>
-      </c>
-      <c r="L11">
-        <v>620</v>
-      </c>
-      <c r="M11">
-        <v>5</v>
-      </c>
-      <c r="N11">
-        <v>7</v>
-      </c>
-      <c r="O11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" t="s">
-        <v>41</v>
       </c>
       <c r="E12">
         <v>8</v>
@@ -1163,13 +1365,13 @@
         <v>13</v>
       </c>
       <c r="J12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K12">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="L12">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="M12">
         <v>8</v>
@@ -1178,15 +1380,21 @@
         <v>9</v>
       </c>
       <c r="O12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="P12" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>11</v>
       </c>
       <c r="D13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E13">
         <v>11</v>
@@ -1204,30 +1412,27 @@
         <v>13</v>
       </c>
       <c r="J13" t="s">
+        <v>99</v>
+      </c>
+      <c r="M13">
+        <v>6</v>
+      </c>
+      <c r="N13">
+        <v>8</v>
+      </c>
+      <c r="P13" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" t="s">
         <v>44</v>
-      </c>
-      <c r="K13">
-        <v>400</v>
-      </c>
-      <c r="L13">
-        <v>1000</v>
-      </c>
-      <c r="M13">
-        <v>8</v>
-      </c>
-      <c r="N13">
-        <v>9</v>
-      </c>
-      <c r="O13" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" t="s">
-        <v>45</v>
       </c>
       <c r="E14">
         <v>8</v>
@@ -1245,13 +1450,13 @@
         <v>13</v>
       </c>
       <c r="J14" t="s">
-        <v>46</v>
+        <v>97</v>
       </c>
       <c r="K14">
-        <v>320</v>
+        <v>800</v>
       </c>
       <c r="L14">
-        <v>600</v>
+        <v>5000</v>
       </c>
       <c r="M14">
         <v>8</v>
@@ -1260,15 +1465,21 @@
         <v>9</v>
       </c>
       <c r="O14" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="P14" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>11</v>
       </c>
       <c r="D15" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E15">
         <v>6</v>
@@ -1286,7 +1497,7 @@
         <v>13</v>
       </c>
       <c r="J15" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K15">
         <v>160</v>
@@ -1301,15 +1512,21 @@
         <v>9</v>
       </c>
       <c r="O15" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="P15" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>11</v>
       </c>
       <c r="D16" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E16">
         <v>6</v>
@@ -1333,7 +1550,7 @@
         <v>1000</v>
       </c>
       <c r="L16">
-        <v>1500</v>
+        <v>3000</v>
       </c>
       <c r="M16">
         <v>8</v>
@@ -1342,15 +1559,21 @@
         <v>9</v>
       </c>
       <c r="O16" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="17" spans="3:15" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="P16" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="17" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>11</v>
       </c>
       <c r="D17" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E17">
         <v>11</v>
@@ -1368,30 +1591,27 @@
         <v>13</v>
       </c>
       <c r="J17" t="s">
-        <v>54</v>
-      </c>
-      <c r="K17">
-        <v>1000</v>
-      </c>
-      <c r="L17">
-        <v>3000</v>
+        <v>53</v>
       </c>
       <c r="M17">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="N17">
         <v>9</v>
       </c>
-      <c r="O17" t="s">
+      <c r="P17" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="18" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="18" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" t="s">
-        <v>55</v>
       </c>
       <c r="E18">
         <v>8</v>
@@ -1409,21 +1629,36 @@
         <v>13</v>
       </c>
       <c r="J18" t="s">
+        <v>55</v>
+      </c>
+      <c r="K18">
+        <v>3</v>
+      </c>
+      <c r="L18">
+        <v>500</v>
+      </c>
+      <c r="M18">
+        <v>6</v>
+      </c>
+      <c r="N18">
+        <v>7</v>
+      </c>
+      <c r="O18" t="s">
         <v>56</v>
       </c>
-      <c r="M18">
-        <v>7</v>
-      </c>
-      <c r="N18">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="P18" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="19" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>11</v>
       </c>
       <c r="D19" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E19">
         <v>6</v>
@@ -1444,7 +1679,7 @@
         <v>58</v>
       </c>
       <c r="K19">
-        <v>3</v>
+        <v>125</v>
       </c>
       <c r="L19">
         <v>500</v>
@@ -1456,15 +1691,21 @@
         <v>7</v>
       </c>
       <c r="O19" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="20" spans="3:15" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="P19" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q19" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="20" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>11</v>
       </c>
       <c r="D20" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E20">
         <v>6</v>
@@ -1484,28 +1725,13 @@
       <c r="J20" t="s">
         <v>61</v>
       </c>
-      <c r="K20">
-        <v>125</v>
-      </c>
-      <c r="L20">
-        <v>500</v>
-      </c>
-      <c r="M20">
-        <v>6</v>
-      </c>
-      <c r="N20">
-        <v>7</v>
-      </c>
-      <c r="O20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="21" spans="3:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
         <v>11</v>
       </c>
       <c r="D21" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E21">
         <v>5</v>
@@ -1526,12 +1752,12 @@
         <v>63</v>
       </c>
     </row>
-    <row r="22" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>11</v>
       </c>
       <c r="D22" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E22">
         <v>12</v>
@@ -1552,12 +1778,12 @@
         <v>65</v>
       </c>
     </row>
-    <row r="23" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
         <v>11</v>
       </c>
       <c r="D23" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E23">
         <v>8</v>
@@ -1578,12 +1804,12 @@
         <v>67</v>
       </c>
     </row>
-    <row r="24" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>11</v>
       </c>
       <c r="D24" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E24">
         <v>6</v>
@@ -1604,12 +1830,12 @@
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>11</v>
       </c>
       <c r="D25" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E25">
         <v>5</v>
@@ -1630,12 +1856,12 @@
         <v>71</v>
       </c>
     </row>
-    <row r="26" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
         <v>11</v>
       </c>
       <c r="D26" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E26">
         <v>5</v>
@@ -1656,12 +1882,12 @@
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
         <v>11</v>
       </c>
       <c r="D27" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E27">
         <v>5</v>
@@ -1682,12 +1908,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="28" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
         <v>11</v>
       </c>
       <c r="D28" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E28">
         <v>5</v>
@@ -1708,12 +1934,12 @@
         <v>77</v>
       </c>
     </row>
-    <row r="29" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
         <v>11</v>
       </c>
       <c r="D29" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E29">
         <v>6</v>
@@ -1727,19 +1953,13 @@
       <c r="H29">
         <v>1.25</v>
       </c>
-      <c r="I29" t="s">
-        <v>13</v>
-      </c>
-      <c r="J29" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="30" spans="3:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
         <v>11</v>
       </c>
       <c r="D30" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E30">
         <v>5</v>
@@ -1753,19 +1973,13 @@
       <c r="H30">
         <v>1.25</v>
       </c>
-      <c r="I30" t="s">
-        <v>13</v>
-      </c>
-      <c r="J30" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="31" spans="3:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
         <v>11</v>
       </c>
       <c r="D31" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E31">
         <v>5</v>
@@ -1779,22 +1993,16 @@
       <c r="H31">
         <v>1.25</v>
       </c>
-      <c r="I31" t="s">
-        <v>13</v>
-      </c>
-      <c r="J31" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="32" spans="3:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
         <v>11</v>
       </c>
       <c r="D32" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E32" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="G32">
         <v>6.3</v>
@@ -1808,10 +2016,10 @@
         <v>11</v>
       </c>
       <c r="D33" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E33" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="G33">
         <v>6.3</v>
@@ -1825,10 +2033,10 @@
         <v>11</v>
       </c>
       <c r="D34" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="E34" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="G34">
         <v>3.2</v>
@@ -1842,10 +2050,10 @@
         <v>11</v>
       </c>
       <c r="D35" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E35" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="G35">
         <v>1.6</v>
@@ -1859,10 +2067,10 @@
         <v>11</v>
       </c>
       <c r="D36" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="E36" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="G36">
         <v>1.6</v>
@@ -1876,10 +2084,10 @@
         <v>11</v>
       </c>
       <c r="D37" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E37" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="G37">
         <v>1.6</v>
@@ -1893,10 +2101,10 @@
         <v>11</v>
       </c>
       <c r="D38" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="E38" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="G38">
         <v>0.8</v>
@@ -1914,67 +2122,94 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L48"/>
+  <dimension ref="A1:R68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="I16" workbookViewId="0">
+      <selection activeCell="O39" sqref="O39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="12" max="12" width="16.77734375" customWidth="1"/>
+    <col min="13" max="13" width="19.88671875" customWidth="1"/>
+    <col min="14" max="14" width="11.109375" customWidth="1"/>
+    <col min="15" max="15" width="19.5546875" customWidth="1"/>
+    <col min="17" max="17" width="11.6640625" customWidth="1"/>
+    <col min="18" max="18" width="15.33203125" customWidth="1"/>
+    <col min="19" max="19" width="23.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C1" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="E1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="F1" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="G1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="H1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="I1" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="J1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="K1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="L1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+      <c r="M1" t="s">
+        <v>90</v>
+      </c>
+      <c r="N1" t="s">
+        <v>91</v>
+      </c>
+      <c r="O1" t="s">
+        <v>92</v>
+      </c>
+      <c r="P1" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>91</v>
+      </c>
+      <c r="R1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D2" t="s">
         <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F2" t="s">
         <v>27</v>
@@ -1983,7 +2218,7 @@
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="I2" t="s">
         <v>10</v>
@@ -1992,27 +2227,45 @@
         <v>12</v>
       </c>
       <c r="K2" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="L2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" t="s">
+        <v>122</v>
+      </c>
+      <c r="O2" t="s">
+        <v>105</v>
+      </c>
+      <c r="P2" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>126</v>
+      </c>
+      <c r="R2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D3" t="s">
         <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F3" t="s">
         <v>12</v>
@@ -2021,7 +2274,7 @@
         <v>27</v>
       </c>
       <c r="H3" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="I3" t="s">
         <v>10</v>
@@ -2030,36 +2283,54 @@
         <v>12</v>
       </c>
       <c r="K3" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="L3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M3" t="s">
+        <v>14</v>
+      </c>
+      <c r="N3" t="s">
+        <v>122</v>
+      </c>
+      <c r="O3" t="s">
+        <v>106</v>
+      </c>
+      <c r="P3" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>126</v>
+      </c>
+      <c r="R3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D4" t="s">
         <v>21</v>
       </c>
       <c r="E4" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F4" t="s">
         <v>17</v>
       </c>
       <c r="G4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H4" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="I4" t="s">
         <v>16</v>
@@ -2068,36 +2339,54 @@
         <v>12</v>
       </c>
       <c r="K4" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="L4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M4" t="s">
+        <v>14</v>
+      </c>
+      <c r="N4" t="s">
+        <v>122</v>
+      </c>
+      <c r="O4" t="s">
+        <v>107</v>
+      </c>
+      <c r="P4" t="s">
+        <v>129</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>126</v>
+      </c>
+      <c r="R4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D5" t="s">
         <v>24</v>
       </c>
       <c r="E5" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F5" t="s">
         <v>21</v>
       </c>
       <c r="G5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H5" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="I5" t="s">
         <v>16</v>
@@ -2106,36 +2395,54 @@
         <v>17</v>
       </c>
       <c r="K5" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="L5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M5" t="s">
+        <v>14</v>
+      </c>
+      <c r="N5" t="s">
+        <v>122</v>
+      </c>
+      <c r="O5" t="s">
+        <v>108</v>
+      </c>
+      <c r="P5" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>126</v>
+      </c>
+      <c r="R5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D6" t="s">
         <v>30</v>
       </c>
       <c r="E6" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F6" t="s">
         <v>27</v>
       </c>
       <c r="G6" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H6" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="I6" t="s">
         <v>16</v>
@@ -2144,36 +2451,54 @@
         <v>17</v>
       </c>
       <c r="K6" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="L6" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M6" t="s">
+        <v>14</v>
+      </c>
+      <c r="N6" t="s">
+        <v>122</v>
+      </c>
+      <c r="O6" t="s">
+        <v>109</v>
+      </c>
+      <c r="P6" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>126</v>
+      </c>
+      <c r="R6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D7" t="s">
         <v>30</v>
       </c>
       <c r="E7" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F7" t="s">
         <v>12</v>
       </c>
       <c r="G7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H7" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="I7" t="s">
         <v>16</v>
@@ -2182,27 +2507,45 @@
         <v>17</v>
       </c>
       <c r="K7" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="L7" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M7" t="s">
+        <v>14</v>
+      </c>
+      <c r="N7" t="s">
+        <v>122</v>
+      </c>
+      <c r="O7" t="s">
+        <v>110</v>
+      </c>
+      <c r="P7" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>126</v>
+      </c>
+      <c r="R7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D8" t="s">
         <v>32</v>
       </c>
       <c r="E8" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F8" t="s">
         <v>30</v>
@@ -2211,85 +2554,112 @@
         <v>21</v>
       </c>
       <c r="K8" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="L8" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M8" t="s">
+        <v>18</v>
+      </c>
+      <c r="N8" t="s">
+        <v>122</v>
+      </c>
+      <c r="O8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C9" t="s">
         <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E9" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="J9" t="s">
         <v>21</v>
       </c>
       <c r="K9" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="L9" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M9" t="s">
+        <v>18</v>
+      </c>
+      <c r="N9" t="s">
+        <v>122</v>
+      </c>
+      <c r="O9" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C10" t="s">
         <v>30</v>
       </c>
       <c r="D10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E10" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J10" t="s">
         <v>21</v>
       </c>
       <c r="K10" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="L10" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M10" t="s">
+        <v>18</v>
+      </c>
+      <c r="N10" t="s">
+        <v>122</v>
+      </c>
+      <c r="O10" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C11" t="s">
         <v>27</v>
       </c>
       <c r="D11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E11" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F11" t="s">
         <v>30</v>
@@ -2298,56 +2668,74 @@
         <v>24</v>
       </c>
       <c r="K11" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="L11" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="M11" t="s">
+        <v>22</v>
+      </c>
+      <c r="N11" t="s">
+        <v>122</v>
+      </c>
+      <c r="O11" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C12" t="s">
         <v>24</v>
       </c>
       <c r="D12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E12" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J12" t="s">
         <v>27</v>
       </c>
       <c r="K12" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="L12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="M12" t="s">
+        <v>22</v>
+      </c>
+      <c r="N12" t="s">
+        <v>122</v>
+      </c>
+      <c r="O12" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C13" t="s">
         <v>21</v>
       </c>
       <c r="D13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E13" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F13" t="s">
         <v>27</v>
@@ -2356,27 +2744,36 @@
         <v>30</v>
       </c>
       <c r="K13" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="L13" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="M13" t="s">
+        <v>22</v>
+      </c>
+      <c r="N13" t="s">
+        <v>122</v>
+      </c>
+      <c r="O13" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C14" t="s">
         <v>17</v>
       </c>
       <c r="D14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E14" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F14" t="s">
         <v>12</v>
@@ -2385,843 +2782,1297 @@
         <v>32</v>
       </c>
       <c r="K14" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="L14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="M14" t="s">
+        <v>25</v>
+      </c>
+      <c r="N14" t="s">
+        <v>122</v>
+      </c>
+      <c r="O14" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>10</v>
       </c>
       <c r="B15" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C15" t="s">
         <v>12</v>
       </c>
       <c r="D15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E15" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J15" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="K15" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="L15" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="M15" t="s">
+        <v>25</v>
+      </c>
+      <c r="N15" t="s">
+        <v>122</v>
+      </c>
+      <c r="O15" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C16" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E16" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J16" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="K16" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="L16" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="M16" t="s">
+        <v>25</v>
+      </c>
+      <c r="N16" t="s">
+        <v>122</v>
+      </c>
+      <c r="O16" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C17" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E17" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J17" t="s">
+        <v>32</v>
+      </c>
+      <c r="K17" t="s">
+        <v>96</v>
+      </c>
+      <c r="L17" t="s">
         <v>34</v>
       </c>
-      <c r="K17" t="s">
-        <v>101</v>
-      </c>
-      <c r="L17" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M17" t="s">
+        <v>123</v>
+      </c>
+      <c r="N17" t="s">
+        <v>122</v>
+      </c>
+      <c r="O17" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C18" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D18" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E18" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F18" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J18" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="K18" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="L18" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="M18" t="s">
+        <v>41</v>
+      </c>
+      <c r="N18" t="s">
+        <v>122</v>
+      </c>
+      <c r="O18" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C19" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D19" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E19" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F19" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="J19" t="s">
+        <v>30</v>
+      </c>
+      <c r="K19" t="s">
+        <v>96</v>
+      </c>
+      <c r="L19" t="s">
         <v>37</v>
       </c>
-      <c r="K19" t="s">
-        <v>101</v>
-      </c>
-      <c r="L19" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M19" t="s">
+        <v>41</v>
+      </c>
+      <c r="N19" t="s">
+        <v>122</v>
+      </c>
+      <c r="O19" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C20" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D20" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E20" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F20" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="J20" t="s">
+        <v>32</v>
+      </c>
+      <c r="K20" t="s">
+        <v>96</v>
+      </c>
+      <c r="L20" t="s">
         <v>37</v>
       </c>
-      <c r="K20" t="s">
-        <v>101</v>
-      </c>
-      <c r="L20" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M20" t="s">
+        <v>41</v>
+      </c>
+      <c r="N20" t="s">
+        <v>122</v>
+      </c>
+      <c r="O20" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>16</v>
       </c>
       <c r="B21" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C21" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D21" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E21" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F21" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="J21" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="K21" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="L21" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="M21" t="s">
+        <v>41</v>
+      </c>
+      <c r="N21" t="s">
+        <v>122</v>
+      </c>
+      <c r="O21" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>16</v>
       </c>
       <c r="B22" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C22" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D22" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E22" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F22" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="J22" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="K22" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="L22" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="M22" t="s">
+        <v>43</v>
+      </c>
+      <c r="N22" t="s">
+        <v>122</v>
+      </c>
+      <c r="O22" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>16</v>
       </c>
       <c r="B23" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C23" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D23" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E23" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F23" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="J23" t="s">
+        <v>32</v>
+      </c>
+      <c r="K23" t="s">
+        <v>96</v>
+      </c>
+      <c r="L23" t="s">
+        <v>28</v>
+      </c>
+      <c r="M23" t="s">
         <v>43</v>
       </c>
-      <c r="K23" t="s">
-        <v>101</v>
-      </c>
-      <c r="L23" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N23" t="s">
+        <v>122</v>
+      </c>
+      <c r="O23" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>16</v>
       </c>
       <c r="B24" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C24" t="s">
+        <v>59</v>
+      </c>
+      <c r="D24" t="s">
+        <v>64</v>
+      </c>
+      <c r="E24" t="s">
+        <v>94</v>
+      </c>
+      <c r="F24" t="s">
         <v>62</v>
       </c>
-      <c r="D24" t="s">
-        <v>68</v>
-      </c>
-      <c r="E24" t="s">
-        <v>99</v>
-      </c>
-      <c r="F24" t="s">
-        <v>66</v>
-      </c>
       <c r="J24" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="K24" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="L24" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="M24" t="s">
+        <v>43</v>
+      </c>
+      <c r="N24" t="s">
+        <v>122</v>
+      </c>
+      <c r="O24" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>16</v>
       </c>
       <c r="B25" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C25" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D25" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E25" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J25" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="K25" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="L25" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+      <c r="M25" t="s">
+        <v>43</v>
+      </c>
+      <c r="N25" t="s">
+        <v>122</v>
+      </c>
+      <c r="O25" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>16</v>
       </c>
       <c r="B26" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C26" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D26" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E26" t="s">
+        <v>94</v>
+      </c>
+      <c r="F26" t="s">
+        <v>36</v>
+      </c>
+      <c r="J26" t="s">
+        <v>36</v>
+      </c>
+      <c r="K26" t="s">
+        <v>96</v>
+      </c>
+      <c r="L26" t="s">
+        <v>55</v>
+      </c>
+      <c r="M26" t="s">
         <v>99</v>
       </c>
-      <c r="F26" t="s">
-        <v>37</v>
-      </c>
-      <c r="J26" t="s">
-        <v>50</v>
-      </c>
-      <c r="K26" t="s">
-        <v>101</v>
-      </c>
-      <c r="L26" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N26" t="s">
+        <v>122</v>
+      </c>
+      <c r="O26" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>16</v>
       </c>
       <c r="B27" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C27" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D27" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E27" t="s">
+        <v>94</v>
+      </c>
+      <c r="F27" t="s">
+        <v>64</v>
+      </c>
+      <c r="J27" t="s">
+        <v>36</v>
+      </c>
+      <c r="K27" t="s">
+        <v>96</v>
+      </c>
+      <c r="L27" t="s">
+        <v>58</v>
+      </c>
+      <c r="M27" t="s">
         <v>99</v>
       </c>
-      <c r="F27" t="s">
-        <v>68</v>
-      </c>
-      <c r="J27" t="s">
-        <v>53</v>
-      </c>
-      <c r="K27" t="s">
-        <v>101</v>
-      </c>
-      <c r="L27" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N27" t="s">
+        <v>122</v>
+      </c>
+      <c r="O27" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>16</v>
       </c>
       <c r="B28" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C28" t="s">
+        <v>50</v>
+      </c>
+      <c r="D28" t="s">
+        <v>70</v>
+      </c>
+      <c r="E28" t="s">
+        <v>94</v>
+      </c>
+      <c r="F28" t="s">
+        <v>36</v>
+      </c>
+      <c r="J28" t="s">
+        <v>38</v>
+      </c>
+      <c r="K28" t="s">
+        <v>96</v>
+      </c>
+      <c r="L28" t="s">
         <v>53</v>
       </c>
-      <c r="D28" t="s">
-        <v>74</v>
-      </c>
-      <c r="E28" t="s">
+      <c r="M28" t="s">
         <v>99</v>
       </c>
-      <c r="F28" t="s">
-        <v>37</v>
-      </c>
-      <c r="J28" t="s">
-        <v>55</v>
-      </c>
-      <c r="K28" t="s">
-        <v>101</v>
-      </c>
-      <c r="L28" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N28" t="s">
+        <v>122</v>
+      </c>
+      <c r="O28" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>16</v>
       </c>
       <c r="B29" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C29" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D29" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E29" t="s">
+        <v>94</v>
+      </c>
+      <c r="F29" t="s">
+        <v>64</v>
+      </c>
+      <c r="J29" t="s">
+        <v>40</v>
+      </c>
+      <c r="K29" t="s">
+        <v>96</v>
+      </c>
+      <c r="L29" t="s">
+        <v>53</v>
+      </c>
+      <c r="M29" t="s">
         <v>99</v>
       </c>
-      <c r="F29" t="s">
-        <v>68</v>
-      </c>
-      <c r="J29" t="s">
-        <v>57</v>
-      </c>
-      <c r="K29" t="s">
-        <v>101</v>
-      </c>
-      <c r="L29" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N29" t="s">
+        <v>122</v>
+      </c>
+      <c r="O29" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>16</v>
       </c>
       <c r="B30" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C30" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D30" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E30" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F30" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="J30" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="K30" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="L30" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="M30" t="s">
+        <v>97</v>
+      </c>
+      <c r="N30" t="s">
+        <v>122</v>
+      </c>
+      <c r="O30" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>16</v>
       </c>
       <c r="B31" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C31" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D31" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E31" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F31" t="s">
         <v>32</v>
       </c>
       <c r="J31" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="K31" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="L31" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="M31" t="s">
+        <v>97</v>
+      </c>
+      <c r="N31" t="s">
+        <v>122</v>
+      </c>
+      <c r="O31" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>16</v>
       </c>
       <c r="B32" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C32" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D32" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E32" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F32" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J32" t="s">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="K32" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="L32" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+      <c r="M32" t="s">
+        <v>97</v>
+      </c>
+      <c r="N32" t="s">
+        <v>122</v>
+      </c>
+      <c r="O32" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>16</v>
       </c>
       <c r="B33" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C33" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D33" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E33" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F33" t="s">
         <v>12</v>
       </c>
       <c r="J33" t="s">
-        <v>66</v>
+        <v>44</v>
       </c>
       <c r="K33" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="L33" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+      <c r="M33" t="s">
+        <v>97</v>
+      </c>
+      <c r="N33" t="s">
+        <v>122</v>
+      </c>
+      <c r="O33" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>16</v>
       </c>
       <c r="B34" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C34" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D34" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E34" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F34" t="s">
         <v>12</v>
       </c>
       <c r="J34" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="K34" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="L34" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="M34" t="s">
+        <v>53</v>
+      </c>
+      <c r="N34" t="s">
+        <v>122</v>
+      </c>
+      <c r="O34" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>16</v>
       </c>
       <c r="B35" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C35" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J35" t="s">
-        <v>70</v>
+        <v>44</v>
       </c>
       <c r="K35" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="L35" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="M35" t="s">
+        <v>53</v>
+      </c>
+      <c r="N35" t="s">
+        <v>122</v>
+      </c>
+      <c r="O35" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>16</v>
       </c>
       <c r="B36" t="s">
+        <v>93</v>
+      </c>
+      <c r="C36" t="s">
+        <v>33</v>
+      </c>
+      <c r="J36" t="s">
+        <v>45</v>
+      </c>
+      <c r="K36" t="s">
+        <v>96</v>
+      </c>
+      <c r="L36" t="s">
         <v>98</v>
       </c>
-      <c r="C36" t="s">
-        <v>34</v>
-      </c>
-      <c r="J36" t="s">
-        <v>72</v>
-      </c>
-      <c r="K36" t="s">
-        <v>101</v>
-      </c>
-      <c r="L36" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M36" t="s">
+        <v>55</v>
+      </c>
+      <c r="N36" t="s">
+        <v>122</v>
+      </c>
+      <c r="O36" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>20</v>
       </c>
       <c r="B37" t="s">
+        <v>93</v>
+      </c>
+      <c r="C37" t="s">
+        <v>42</v>
+      </c>
+      <c r="J37" t="s">
+        <v>48</v>
+      </c>
+      <c r="K37" t="s">
+        <v>96</v>
+      </c>
+      <c r="L37" t="s">
         <v>98</v>
       </c>
-      <c r="C37" t="s">
-        <v>43</v>
-      </c>
-      <c r="J37" t="s">
-        <v>74</v>
-      </c>
-      <c r="K37" t="s">
-        <v>101</v>
-      </c>
-      <c r="L37" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M37" t="s">
+        <v>58</v>
+      </c>
+      <c r="N37" t="s">
+        <v>122</v>
+      </c>
+      <c r="O37" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>23</v>
       </c>
       <c r="B38" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="J38" t="s">
-        <v>76</v>
+        <v>50</v>
       </c>
       <c r="K38" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="L38" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="M38" t="s">
+        <v>124</v>
+      </c>
+      <c r="N38" t="s">
+        <v>122</v>
+      </c>
+      <c r="O38" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>23</v>
       </c>
       <c r="B39" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C39" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="J39" t="s">
-        <v>78</v>
+        <v>52</v>
       </c>
       <c r="K39" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="L39" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="M39" t="s">
+        <v>51</v>
+      </c>
+      <c r="N39" t="s">
+        <v>122</v>
+      </c>
+      <c r="O39" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>26</v>
       </c>
       <c r="B40" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C40" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="J40" t="s">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="K40" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="L40" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>26</v>
       </c>
       <c r="B41" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C41" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="J41" t="s">
-        <v>82</v>
+        <v>52</v>
       </c>
       <c r="K41" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="L41" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>26</v>
       </c>
       <c r="B42" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C42" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="J42" t="s">
-        <v>84</v>
+        <v>54</v>
       </c>
       <c r="K42" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="L42" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>26</v>
       </c>
       <c r="B43" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C43" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="J43" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="K43" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="L43" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>26</v>
       </c>
       <c r="B44" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C44" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="J44" t="s">
-        <v>88</v>
+        <v>59</v>
       </c>
       <c r="K44" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="L44" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>26</v>
       </c>
       <c r="B45" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C45" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="J45" t="s">
-        <v>89</v>
+        <v>60</v>
       </c>
       <c r="K45" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="L45" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="J46" t="s">
-        <v>91</v>
+        <v>62</v>
       </c>
       <c r="K46" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="L46" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="J47" t="s">
-        <v>92</v>
+        <v>64</v>
       </c>
       <c r="K47" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="L47" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J48" t="s">
+        <v>66</v>
+      </c>
+      <c r="K48" t="s">
+        <v>96</v>
+      </c>
+      <c r="L48" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="49" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="J49" t="s">
+        <v>68</v>
+      </c>
+      <c r="K49" t="s">
+        <v>96</v>
+      </c>
+      <c r="L49" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="50" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="J50" t="s">
+        <v>70</v>
+      </c>
+      <c r="K50" t="s">
+        <v>96</v>
+      </c>
+      <c r="L50" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="51" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="J51" t="s">
+        <v>72</v>
+      </c>
+      <c r="K51" t="s">
+        <v>96</v>
+      </c>
+      <c r="L51" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="52" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="J52" t="s">
+        <v>74</v>
+      </c>
+      <c r="K52" t="s">
+        <v>96</v>
+      </c>
+      <c r="L52" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="53" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="J53" t="s">
+        <v>76</v>
+      </c>
+      <c r="K53" t="s">
+        <v>96</v>
+      </c>
+      <c r="L53" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="54" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="J54" t="s">
+        <v>78</v>
+      </c>
+      <c r="K54" t="s">
+        <v>96</v>
+      </c>
+      <c r="L54" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="55" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="J55" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="J48" t="s">
-        <v>93</v>
-      </c>
-      <c r="K48" t="s">
-        <v>101</v>
-      </c>
-      <c r="L48" t="s">
+      <c r="K55" t="s">
+        <v>96</v>
+      </c>
+      <c r="L55" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="56" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="J56" t="s">
         <v>81</v>
+      </c>
+      <c r="K56" t="s">
+        <v>96</v>
+      </c>
+      <c r="L56" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="57" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="J57" t="s">
+        <v>83</v>
+      </c>
+      <c r="K57" t="s">
+        <v>96</v>
+      </c>
+      <c r="L57" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="58" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="J58" t="s">
+        <v>84</v>
+      </c>
+      <c r="K58" t="s">
+        <v>96</v>
+      </c>
+      <c r="L58" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="59" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="J59" t="s">
+        <v>86</v>
+      </c>
+      <c r="K59" t="s">
+        <v>96</v>
+      </c>
+      <c r="L59" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="60" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="J60" t="s">
+        <v>87</v>
+      </c>
+      <c r="K60" t="s">
+        <v>96</v>
+      </c>
+      <c r="L60" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="61" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="J61" t="s">
+        <v>88</v>
+      </c>
+      <c r="K61" t="s">
+        <v>96</v>
+      </c>
+      <c r="L61" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="62" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="J62" t="s">
+        <v>79</v>
+      </c>
+      <c r="K62" t="s">
+        <v>96</v>
+      </c>
+      <c r="L62" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="63" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="J63" t="s">
+        <v>81</v>
+      </c>
+      <c r="K63" t="s">
+        <v>96</v>
+      </c>
+      <c r="L63" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="64" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="J64" t="s">
+        <v>83</v>
+      </c>
+      <c r="K64" t="s">
+        <v>96</v>
+      </c>
+      <c r="L64" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="65" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="J65" t="s">
+        <v>84</v>
+      </c>
+      <c r="K65" t="s">
+        <v>96</v>
+      </c>
+      <c r="L65" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="66" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="J66" t="s">
+        <v>86</v>
+      </c>
+      <c r="K66" t="s">
+        <v>96</v>
+      </c>
+      <c r="L66" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="67" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="J67" t="s">
+        <v>87</v>
+      </c>
+      <c r="K67" t="s">
+        <v>96</v>
+      </c>
+      <c r="L67" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="68" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="J68" t="s">
+        <v>88</v>
+      </c>
+      <c r="K68" t="s">
+        <v>96</v>
+      </c>
+      <c r="L68" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add fixture node and its relatstionship
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\1 学习资料\9-大四上\制造工艺设计实践\202221106-knowlegeGraph\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F45B2C3B-1C8A-40A1-A4B3-E02886F7323F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC2F49A6-54A6-4FCE-B2A2-815296DDB08F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8184" yWindow="156" windowWidth="12156" windowHeight="12192" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="96" yWindow="300" windowWidth="12792" windowHeight="11796" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="nodeData" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="881" uniqueCount="146">
   <si>
     <t>label</t>
   </si>
@@ -453,6 +453,56 @@
   </si>
   <si>
     <t>精拉</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fixture</t>
+  </si>
+  <si>
+    <t>顶尖</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>鸡心卡头</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>卡环</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>快换卡头</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>拨盘</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>花盘</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>三爪拨盘</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>三爪卡盘</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>四爪卡盘</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>滑柱钻模</t>
+  </si>
+  <si>
+    <t>装备夹具</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>钻模</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -460,7 +510,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -478,6 +528,12 @@
     <font>
       <sz val="8"/>
       <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF010E1F"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -502,9 +558,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -785,10 +842,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q38"/>
+  <dimension ref="A1:S38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="Q19" sqref="Q19"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18:J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -801,7 +858,7 @@
     <col min="17" max="17" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -853,8 +910,14 @@
       <c r="Q1" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R1" t="s">
+        <v>102</v>
+      </c>
+      <c r="S1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -906,8 +969,14 @@
       <c r="Q2" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R2" t="s">
+        <v>133</v>
+      </c>
+      <c r="S2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -959,8 +1028,14 @@
       <c r="Q3" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R3" t="s">
+        <v>133</v>
+      </c>
+      <c r="S3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1012,8 +1087,14 @@
       <c r="Q4" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R4" t="s">
+        <v>133</v>
+      </c>
+      <c r="S4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1065,8 +1146,14 @@
       <c r="Q5" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R5" t="s">
+        <v>133</v>
+      </c>
+      <c r="S5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1118,8 +1205,14 @@
       <c r="Q6" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R6" t="s">
+        <v>133</v>
+      </c>
+      <c r="S6" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>11</v>
       </c>
@@ -1165,8 +1258,14 @@
       <c r="Q7" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R7" t="s">
+        <v>133</v>
+      </c>
+      <c r="S7" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>11</v>
       </c>
@@ -1206,8 +1305,14 @@
       <c r="Q8" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R8" t="s">
+        <v>133</v>
+      </c>
+      <c r="S8" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>11</v>
       </c>
@@ -1247,8 +1352,14 @@
       <c r="Q9" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R9" t="s">
+        <v>133</v>
+      </c>
+      <c r="S9" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>11</v>
       </c>
@@ -1294,8 +1405,14 @@
       <c r="Q10" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R10" t="s">
+        <v>133</v>
+      </c>
+      <c r="S10" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>11</v>
       </c>
@@ -1341,8 +1458,14 @@
       <c r="Q11" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R11" t="s">
+        <v>133</v>
+      </c>
+      <c r="S11" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>11</v>
       </c>
@@ -1389,7 +1512,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>11</v>
       </c>
@@ -1427,7 +1550,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>11</v>
       </c>
@@ -1474,7 +1597,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>11</v>
       </c>
@@ -1521,7 +1644,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>11</v>
       </c>
@@ -2122,10 +2245,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:R68"/>
+  <dimension ref="A1:U68"/>
   <sheetViews>
-    <sheetView topLeftCell="I16" workbookViewId="0">
-      <selection activeCell="O39" sqref="O39"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="T9" sqref="T9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2136,10 +2259,11 @@
     <col min="15" max="15" width="19.5546875" customWidth="1"/>
     <col min="17" max="17" width="11.6640625" customWidth="1"/>
     <col min="18" max="18" width="15.33203125" customWidth="1"/>
-    <col min="19" max="19" width="23.6640625" customWidth="1"/>
+    <col min="19" max="19" width="17.44140625" customWidth="1"/>
+    <col min="20" max="20" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>90</v>
       </c>
@@ -2194,8 +2318,17 @@
       <c r="R1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S1" t="s">
+        <v>90</v>
+      </c>
+      <c r="T1" t="s">
+        <v>91</v>
+      </c>
+      <c r="U1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -2250,8 +2383,17 @@
       <c r="R2" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S2" t="s">
+        <v>14</v>
+      </c>
+      <c r="T2" t="s">
+        <v>144</v>
+      </c>
+      <c r="U2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -2306,8 +2448,17 @@
       <c r="R3" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S3" t="s">
+        <v>14</v>
+      </c>
+      <c r="T3" t="s">
+        <v>144</v>
+      </c>
+      <c r="U3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -2362,8 +2513,17 @@
       <c r="R4" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S4" t="s">
+        <v>14</v>
+      </c>
+      <c r="T4" t="s">
+        <v>144</v>
+      </c>
+      <c r="U4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -2418,8 +2578,17 @@
       <c r="R5" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S5" t="s">
+        <v>14</v>
+      </c>
+      <c r="T5" t="s">
+        <v>144</v>
+      </c>
+      <c r="U5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -2474,8 +2643,17 @@
       <c r="R6" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S6" t="s">
+        <v>14</v>
+      </c>
+      <c r="T6" t="s">
+        <v>144</v>
+      </c>
+      <c r="U6" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -2530,8 +2708,17 @@
       <c r="R7" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S7" t="s">
+        <v>14</v>
+      </c>
+      <c r="T7" t="s">
+        <v>144</v>
+      </c>
+      <c r="U7" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -2568,8 +2755,17 @@
       <c r="O8" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S8" t="s">
+        <v>14</v>
+      </c>
+      <c r="T8" t="s">
+        <v>144</v>
+      </c>
+      <c r="U8" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -2606,8 +2802,17 @@
       <c r="O9" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S9" t="s">
+        <v>14</v>
+      </c>
+      <c r="T9" t="s">
+        <v>144</v>
+      </c>
+      <c r="U9" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -2644,8 +2849,17 @@
       <c r="O10" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S10" t="s">
+        <v>14</v>
+      </c>
+      <c r="T10" t="s">
+        <v>144</v>
+      </c>
+      <c r="U10" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -2682,8 +2896,17 @@
       <c r="O11" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S11" t="s">
+        <v>18</v>
+      </c>
+      <c r="T11" t="s">
+        <v>144</v>
+      </c>
+      <c r="U11" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -2720,8 +2943,17 @@
       <c r="O12" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S12" t="s">
+        <v>22</v>
+      </c>
+      <c r="T12" t="s">
+        <v>144</v>
+      </c>
+      <c r="U12" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -2758,8 +2990,17 @@
       <c r="O13" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S13" t="s">
+        <v>25</v>
+      </c>
+      <c r="T13" t="s">
+        <v>144</v>
+      </c>
+      <c r="U13" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -2796,8 +3037,17 @@
       <c r="O14" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S14" t="s">
+        <v>55</v>
+      </c>
+      <c r="T14" t="s">
+        <v>144</v>
+      </c>
+      <c r="U14" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -2834,8 +3084,17 @@
       <c r="O15" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S15" t="s">
+        <v>58</v>
+      </c>
+      <c r="T15" t="s">
+        <v>144</v>
+      </c>
+      <c r="U15" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>

</xml_diff>